<commit_message>
Published state of ETDataset for deploy December 2025
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy/energy_production_biomethanol_to_jet.xlsx
+++ b/nodes_source_analyses/energy/energy/energy_production_biomethanol_to_jet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Github/etdataset/nodes_source_analyses/energy/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A222D-75A9-9B41-9CCE-2225F6F2F1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E15360-79F9-A140-AD41-0548A4EA3AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10380" yWindow="-28300" windowWidth="25600" windowHeight="13660" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19340" yWindow="-28300" windowWidth="25600" windowHeight="27340" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
   <si>
     <t>Source</t>
   </si>
@@ -412,9 +412,6 @@
     <t>heat</t>
   </si>
   <si>
-    <t>kg</t>
-  </si>
-  <si>
     <t>Output products</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>correction light gases</t>
   </si>
   <si>
-    <t>MJ in / MJ out</t>
-  </si>
-  <si>
     <t>Feedstock in- and output</t>
   </si>
   <si>
@@ -442,15 +436,6 @@
     <t>- conversions from kg to MJs</t>
   </si>
   <si>
-    <t>Validation</t>
-  </si>
-  <si>
-    <t>Simplified calculation based only on Concawe &amp; Armaco, to check if calculation results above make sense</t>
-  </si>
-  <si>
-    <t>final correction MJ in / MJ out</t>
-  </si>
-  <si>
     <t>loss</t>
   </si>
   <si>
@@ -532,51 +517,15 @@
     <t>kg/kg biokerosene</t>
   </si>
   <si>
-    <t>corrected kg/kg biokerosene</t>
-  </si>
-  <si>
-    <t>MJ / kg biokerosene</t>
-  </si>
-  <si>
-    <t>MJ/MJ biokerosene</t>
-  </si>
-  <si>
-    <t>kg / kg biokerosene</t>
-  </si>
-  <si>
-    <t>MJ / MJ biokerosene</t>
-  </si>
-  <si>
     <t>input.biomethanol</t>
   </si>
   <si>
     <t>biomethanol</t>
   </si>
   <si>
-    <t>output.bio_ethanol</t>
-  </si>
-  <si>
-    <t>biogasoline</t>
-  </si>
-  <si>
-    <t>note that whereas the output product should be biogasoline, this is not yet a carrier in the ETM. Therefore, the LHV of gasoline from ETSource is taken</t>
-  </si>
-  <si>
-    <t>correction is applied to account for by-products biogasoline and light gases, since Concawe &amp; Aramco only reports fuel fractions based on biokerosene production</t>
-  </si>
-  <si>
-    <t>- allocate light gases output to proportionally increased biokerosene and biogasoline output (light gases difficult to model but have energy purpose)</t>
-  </si>
-  <si>
     <t>- note that in- and output of water is not modelled in the ETM. Therefore, the output of water is ignored</t>
   </si>
   <si>
-    <t xml:space="preserve">assumption: biogasoline is not modelled in the ETM. Instead, the ETM models biogasoline flows from Eurostat energy balance as bioethanol. </t>
-  </si>
-  <si>
-    <t>Therefore, biogasoline production is assumed to be bioethanol production</t>
-  </si>
-  <si>
     <t>output.bio_kerosene</t>
   </si>
   <si>
@@ -584,6 +533,64 @@
   </si>
   <si>
     <t>energy_production_biomethanol_to_jet; note that largely the same assumptions and sources are used as done for energy_production_methanol_to_jet</t>
+  </si>
+  <si>
+    <t>Concawe &amp; Aramco (2022), Wang et al. (2015), expert from Kalavasta</t>
+  </si>
+  <si>
+    <t>output.bionaphtha</t>
+  </si>
+  <si>
+    <t>Assumptions:</t>
+  </si>
+  <si>
+    <t>correction is applied to account for by-products gasoline and light gases, since Concawe &amp; Aramco only reports fuel fractions based on kerosene production</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note that the reported gasoline output from Concawe &amp; Aramco is assumed to be </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>naphtha</t>
+    </r>
+  </si>
+  <si>
+    <t>According to an expert from Kalavasta (maintainer of the CTM), output of gasoline can be considered a product with carbon range similar to gasoline</t>
+  </si>
+  <si>
+    <t>bionaphtha</t>
+  </si>
+  <si>
+    <t>Expert judgement from Kalavasta</t>
+  </si>
+  <si>
+    <t>7-11-2025</t>
+  </si>
+  <si>
+    <t>Output of bionaphtha</t>
+  </si>
+  <si>
+    <t>Concerning assumption of bionaphtha output instead of biogasoline</t>
+  </si>
+  <si>
+    <t>Considering the importance of naphtha in the future compared to decreased importance of gasoline, and considering naphta has a similar carbon range as gasoline, the output is considered to be naphtha</t>
+  </si>
+  <si>
+    <t>conversion to MJ</t>
+  </si>
+  <si>
+    <t>correction heat and electricity</t>
+  </si>
+  <si>
+    <t>- allocate light gases output to proportionally increase biokerosene and bionaphtha output (light gases difficult to model but have energy purpose)</t>
+  </si>
+  <si>
+    <t>normalise on input</t>
   </si>
 </sst>
 </file>
@@ -597,12 +604,26 @@
     <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="35">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -812,8 +833,18 @@
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,6 +915,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1106,582 +1143,601 @@
   </borders>
   <cellStyleXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="27" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="356" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="356" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="20" fillId="2" borderId="0" xfId="357" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="18" fillId="2" borderId="0" xfId="357" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="34" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="357" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="20" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="20" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="20" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="358">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2060,13 +2116,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1351561</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>38382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>793042</xdr:colOff>
       <xdr:row>77</xdr:row>
       <xdr:rowOff>34173</xdr:rowOff>
@@ -2104,13 +2160,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1181612</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>41077</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>172897</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>91877</xdr:rowOff>
@@ -2148,13 +2204,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>231141</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>126490</xdr:rowOff>
@@ -2554,31 +2610,31 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="116" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="117"/>
-      <c r="E4" s="115"/>
+      <c r="C4" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="108"/>
+      <c r="E4" s="106"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="113" t="s">
+      <c r="C5" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="118"/>
+      <c r="D5" s="109"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="114" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="119"/>
+      <c r="C6" s="105" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="110"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
@@ -2596,31 +2652,31 @@
         <v>16</v>
       </c>
       <c r="C9" s="32"/>
-      <c r="D9" s="117"/>
+      <c r="D9" s="108"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="118"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="109"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="121" t="s">
+      <c r="C11" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="118"/>
+      <c r="D11" s="109"/>
     </row>
     <row r="12" spans="1:5" ht="17" thickBot="1">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="118"/>
+      <c r="D12" s="109"/>
     </row>
     <row r="13" spans="1:5" ht="17" thickBot="1">
       <c r="A13" s="1"/>
@@ -2628,91 +2684,91 @@
       <c r="C13" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="118"/>
+      <c r="D13" s="109"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="118"/>
+      <c r="D14" s="109"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="118"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="109"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="118"/>
+      <c r="D16" s="109"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
-      <c r="C17" s="124" t="s">
+      <c r="C17" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="118"/>
+      <c r="D17" s="109"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="118"/>
+      <c r="D18" s="109"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
-      <c r="C19" s="126" t="s">
+      <c r="C19" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="118"/>
+      <c r="D19" s="109"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="B20" s="35"/>
-      <c r="C20" s="127" t="s">
+      <c r="C20" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="118"/>
+      <c r="D20" s="109"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1"/>
       <c r="B21" s="35"/>
-      <c r="C21" s="128" t="s">
+      <c r="C21" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="118"/>
+      <c r="D21" s="109"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1"/>
       <c r="B22" s="35"/>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="118"/>
+      <c r="D22" s="109"/>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" s="35"/>
-      <c r="C23" s="130" t="s">
+      <c r="C23" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="118"/>
+      <c r="D23" s="109"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" s="131"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="119"/>
+      <c r="B24" s="121"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="110"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2728,7 +2784,7 @@
   <dimension ref="B2:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2746,30 +2802,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="106"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="133"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="107"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="109"/>
+      <c r="B3" s="134"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="136"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="107"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="109"/>
+      <c r="B4" s="134"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="136"/>
     </row>
     <row r="5" spans="2:10" ht="31" customHeight="1">
-      <c r="B5" s="110"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="112"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="139"/>
     </row>
     <row r="7" spans="2:10" ht="17" thickBot="1"/>
     <row r="8" spans="2:10">
@@ -2827,33 +2883,33 @@
       </c>
       <c r="E12" s="47">
         <f>ROUND(Notes!C2,3)</f>
-        <v>1660.192</v>
+        <v>1812.096</v>
       </c>
       <c r="F12" s="45"/>
       <c r="G12" s="59"/>
       <c r="H12" s="60"/>
       <c r="I12" s="101" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J12" s="61"/>
     </row>
     <row r="13" spans="2:10" ht="20" thickBot="1">
       <c r="B13" s="58"/>
       <c r="C13" s="102" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="62">
         <f>ROUND(Notes!C6,5)</f>
-        <v>0.95984000000000003</v>
+        <v>0.96028000000000002</v>
       </c>
       <c r="F13" s="45"/>
       <c r="G13" s="59"/>
       <c r="H13" s="60"/>
       <c r="I13" s="101" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J13" s="61"/>
     </row>
@@ -2867,53 +2923,53 @@
       </c>
       <c r="E14" s="62">
         <f>ROUND(Notes!C7,5)</f>
-        <v>4.0160000000000001E-2</v>
+        <v>3.9719999999999998E-2</v>
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="59"/>
       <c r="H14" s="60"/>
       <c r="I14" s="101" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J14" s="61"/>
     </row>
     <row r="15" spans="2:10" ht="17" thickBot="1">
       <c r="B15" s="63"/>
       <c r="C15" s="103" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="62">
         <f>ROUND(Notes!C8,5)</f>
-        <v>0.82399999999999995</v>
+        <v>0.75492999999999999</v>
       </c>
       <c r="F15" s="50"/>
       <c r="G15" s="50"/>
       <c r="H15" s="50"/>
       <c r="I15" s="101" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J15" s="64"/>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1">
       <c r="B16" s="63"/>
-      <c r="C16" s="103" t="s">
-        <v>145</v>
+      <c r="C16" s="124" t="s">
+        <v>140</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="62">
         <f>ROUND(Notes!C9,5)</f>
-        <v>0.15090999999999999</v>
+        <v>0.14402000000000001</v>
       </c>
       <c r="F16" s="50"/>
       <c r="G16" s="50"/>
       <c r="H16" s="50"/>
-      <c r="I16" s="101" t="s">
-        <v>132</v>
+      <c r="I16" s="123" t="s">
+        <v>139</v>
       </c>
       <c r="J16" s="64"/>
     </row>
@@ -2933,7 +2989,7 @@
       <c r="G17" s="45"/>
       <c r="H17" s="66"/>
       <c r="I17" s="101" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J17" s="67"/>
     </row>
@@ -2998,7 +3054,7 @@
       </c>
       <c r="H21" s="50"/>
       <c r="I21" s="101" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J21" s="64"/>
     </row>
@@ -3039,7 +3095,7 @@
       </c>
       <c r="H23" s="50"/>
       <c r="I23" s="101" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J23" s="64"/>
     </row>
@@ -3061,7 +3117,7 @@
       </c>
       <c r="H24" s="51"/>
       <c r="I24" s="101" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J24" s="70"/>
     </row>
@@ -3208,7 +3264,7 @@
       </c>
       <c r="H32" s="50"/>
       <c r="I32" s="101" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J32" s="64"/>
     </row>
@@ -3280,7 +3336,7 @@
   <dimension ref="B1:J34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
@@ -3366,22 +3422,22 @@
     <row r="7" spans="2:10">
       <c r="B7" s="39"/>
       <c r="C7" s="100" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D7" s="100" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F7" s="25">
         <v>2022</v>
       </c>
       <c r="G7" s="100" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H7" s="91" t="s">
         <v>85</v>
       </c>
       <c r="J7" s="92" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -3396,29 +3452,42 @@
     <row r="10" spans="2:10">
       <c r="B10" s="39"/>
       <c r="C10" s="100" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="100" t="s">
         <v>123</v>
-      </c>
-      <c r="D10" s="100" t="s">
-        <v>128</v>
       </c>
       <c r="F10" s="25">
         <v>2016</v>
       </c>
       <c r="G10" s="100" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H10" s="91" t="s">
         <v>85</v>
       </c>
       <c r="J10" s="92" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="39"/>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="39"/>
+    <row r="12" spans="2:10" s="126" customFormat="1">
+      <c r="B12" s="125"/>
+      <c r="C12" s="126" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="126" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="126" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" s="127" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" s="127"/>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="39"/>
@@ -3487,7 +3556,7 @@
       <c r="B34" s="39"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="24" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J7" r:id="rId1" xr:uid="{CA4435BF-7BC0-5946-B941-E72619E47EA7}"/>
     <hyperlink ref="J10" r:id="rId2" xr:uid="{44305025-BB8A-4D46-A44D-6B29F2B5A0C5}"/>
@@ -3502,10 +3571,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:Y85"/>
+  <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -3513,38 +3582,40 @@
     <col min="1" max="1" width="26.1640625" style="29" customWidth="1"/>
     <col min="2" max="2" width="29" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="29" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="25" style="29" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="29" customWidth="1"/>
-    <col min="7" max="10" width="10.6640625" style="29"/>
-    <col min="11" max="11" width="16.1640625" style="29" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="29"/>
-    <col min="13" max="13" width="26.83203125" style="29" customWidth="1"/>
-    <col min="14" max="14" width="26.5" style="29" customWidth="1"/>
-    <col min="15" max="16384" width="10.6640625" style="29"/>
+    <col min="4" max="5" width="19.33203125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="29" customWidth="1"/>
+    <col min="8" max="8" width="25" style="29" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="29" customWidth="1"/>
+    <col min="10" max="13" width="10.6640625" style="29"/>
+    <col min="14" max="14" width="16.1640625" style="29" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="29"/>
+    <col min="16" max="16" width="26.83203125" style="29" customWidth="1"/>
+    <col min="17" max="17" width="26.5" style="29" customWidth="1"/>
+    <col min="18" max="16384" width="10.6640625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25">
+    <row r="1" spans="2:28">
       <c r="B1" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="2:25">
+    <row r="2" spans="2:28">
       <c r="B2" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="41">
         <f>C19</f>
-        <v>1660.1920877257439</v>
+        <v>1812.0956459316621</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="2:25">
+      <c r="P2" s="29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="2:28">
       <c r="B3" s="29" t="s">
         <v>38</v>
       </c>
@@ -3555,10 +3626,10 @@
         <v>39</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="2:25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28">
       <c r="B4" s="29" t="s">
         <v>41</v>
       </c>
@@ -3570,146 +3641,140 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:25">
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
+    <row r="5" spans="2:28">
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
       <c r="R5" s="76"/>
       <c r="S5" s="76"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
+      <c r="T5" s="76"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76"/>
       <c r="W5" s="77"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78"/>
-    </row>
-    <row r="6" spans="2:25">
+      <c r="X5" s="77"/>
+      <c r="Y5" s="77"/>
+      <c r="Z5" s="77"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="78"/>
+    </row>
+    <row r="6" spans="2:28">
       <c r="B6" s="29" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C6" s="37">
-        <f>I53</f>
-        <v>0.95984365433259322</v>
-      </c>
-      <c r="M6" s="75"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
+        <f>G53</f>
+        <v>0.96028477410542445</v>
+      </c>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="79"/>
       <c r="R6" s="77"/>
       <c r="S6" s="77"/>
       <c r="T6" s="77"/>
       <c r="U6" s="77"/>
       <c r="V6" s="77"/>
       <c r="W6" s="77"/>
-      <c r="X6" s="80"/>
-      <c r="Y6" s="80"/>
-    </row>
-    <row r="7" spans="2:25">
+      <c r="X6" s="77"/>
+      <c r="Y6" s="77"/>
+      <c r="Z6" s="77"/>
+      <c r="AA6" s="80"/>
+      <c r="AB6" s="80"/>
+    </row>
+    <row r="7" spans="2:28">
       <c r="B7" s="29" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="37">
-        <f>I54</f>
-        <v>4.0156345667406765E-2</v>
-      </c>
-      <c r="M7" s="81"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="83"/>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="83"/>
+        <f>G54</f>
+        <v>3.9715225894575636E-2</v>
+      </c>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="82"/>
       <c r="R7" s="83"/>
       <c r="S7" s="83"/>
       <c r="T7" s="83"/>
       <c r="U7" s="83"/>
       <c r="V7" s="83"/>
       <c r="W7" s="83"/>
-      <c r="X7" s="84"/>
-      <c r="Y7" s="84"/>
-    </row>
-    <row r="8" spans="2:25">
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="84"/>
+      <c r="AB7" s="84"/>
+    </row>
+    <row r="8" spans="2:28">
       <c r="B8" s="29" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C8" s="37">
-        <f>I58</f>
-        <v>0.82400103585241713</v>
-      </c>
-      <c r="M8" s="85"/>
-      <c r="N8" s="85"/>
-      <c r="O8" s="83"/>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
+        <f>G59</f>
+        <v>0.75492703879693013</v>
+      </c>
+      <c r="P8" s="85"/>
+      <c r="Q8" s="85"/>
       <c r="R8" s="83"/>
       <c r="S8" s="83"/>
       <c r="T8" s="83"/>
       <c r="U8" s="83"/>
       <c r="V8" s="83"/>
       <c r="W8" s="83"/>
-      <c r="X8" s="84"/>
-      <c r="Y8" s="84"/>
-    </row>
-    <row r="9" spans="2:25">
+      <c r="X8" s="83"/>
+      <c r="Y8" s="83"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="84"/>
+      <c r="AB8" s="84"/>
+    </row>
+    <row r="9" spans="2:28">
       <c r="B9" s="29" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C9" s="37">
-        <f>I59</f>
-        <v>0.15090655716936563</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="M9" s="85"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="83"/>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="87"/>
+        <f>G60</f>
+        <v>0.14401711307348949</v>
+      </c>
+      <c r="P9" s="85"/>
+      <c r="Q9" s="86"/>
       <c r="R9" s="83"/>
       <c r="S9" s="83"/>
-      <c r="T9" s="88"/>
-      <c r="U9" s="88"/>
-      <c r="V9" s="88"/>
+      <c r="T9" s="87"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="83"/>
       <c r="W9" s="88"/>
-      <c r="X9" s="84"/>
-      <c r="Y9" s="84"/>
-    </row>
-    <row r="10" spans="2:25">
-      <c r="E10" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="M10" s="85"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="87"/>
+      <c r="X9" s="88"/>
+      <c r="Y9" s="88"/>
+      <c r="Z9" s="88"/>
+      <c r="AA9" s="84"/>
+      <c r="AB9" s="84"/>
+    </row>
+    <row r="10" spans="2:28">
+      <c r="P10" s="85"/>
+      <c r="Q10" s="86"/>
       <c r="R10" s="83"/>
       <c r="S10" s="83"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
+      <c r="T10" s="87"/>
+      <c r="U10" s="83"/>
+      <c r="V10" s="83"/>
       <c r="W10" s="88"/>
-      <c r="X10" s="84"/>
-      <c r="Y10" s="84"/>
-    </row>
-    <row r="11" spans="2:25">
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="87"/>
+      <c r="X10" s="88"/>
+      <c r="Y10" s="88"/>
+      <c r="Z10" s="88"/>
+      <c r="AA10" s="84"/>
+      <c r="AB10" s="84"/>
+    </row>
+    <row r="11" spans="2:28">
+      <c r="P11" s="85"/>
+      <c r="Q11" s="85"/>
       <c r="R11" s="83"/>
       <c r="S11" s="83"/>
-      <c r="T11" s="83"/>
+      <c r="T11" s="87"/>
       <c r="U11" s="83"/>
       <c r="V11" s="83"/>
       <c r="W11" s="83"/>
-      <c r="X11" s="84"/>
-      <c r="Y11" s="84"/>
-    </row>
-    <row r="12" spans="2:25">
+      <c r="X11" s="83"/>
+      <c r="Y11" s="83"/>
+      <c r="Z11" s="83"/>
+      <c r="AA11" s="84"/>
+      <c r="AB11" s="84"/>
+    </row>
+    <row r="12" spans="2:28">
       <c r="B12" s="29" t="s">
         <v>43</v>
       </c>
@@ -3720,21 +3785,21 @@
       <c r="D12" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="M12" s="85"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="87"/>
+      <c r="P12" s="85"/>
+      <c r="Q12" s="86"/>
       <c r="R12" s="83"/>
       <c r="S12" s="83"/>
-      <c r="T12" s="88"/>
-      <c r="U12" s="88"/>
-      <c r="V12" s="88"/>
+      <c r="T12" s="87"/>
+      <c r="U12" s="83"/>
+      <c r="V12" s="83"/>
       <c r="W12" s="88"/>
-      <c r="X12" s="84"/>
-      <c r="Y12" s="84"/>
-    </row>
-    <row r="13" spans="2:25">
+      <c r="X12" s="88"/>
+      <c r="Y12" s="88"/>
+      <c r="Z12" s="88"/>
+      <c r="AA12" s="84"/>
+      <c r="AB12" s="84"/>
+    </row>
+    <row r="13" spans="2:28">
       <c r="B13" s="29" t="s">
         <v>45</v>
       </c>
@@ -3745,21 +3810,21 @@
       <c r="D13" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="M13" s="85"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="87"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="86"/>
       <c r="R13" s="83"/>
       <c r="S13" s="83"/>
-      <c r="T13" s="88"/>
-      <c r="U13" s="88"/>
-      <c r="V13" s="88"/>
+      <c r="T13" s="87"/>
+      <c r="U13" s="83"/>
+      <c r="V13" s="83"/>
       <c r="W13" s="88"/>
-      <c r="X13" s="84"/>
-      <c r="Y13" s="84"/>
-    </row>
-    <row r="14" spans="2:25">
+      <c r="X13" s="88"/>
+      <c r="Y13" s="88"/>
+      <c r="Z13" s="88"/>
+      <c r="AA13" s="84"/>
+      <c r="AB13" s="84"/>
+    </row>
+    <row r="14" spans="2:28">
       <c r="B14" s="29" t="s">
         <v>47</v>
       </c>
@@ -3770,55 +3835,61 @@
       <c r="D14" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="85"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="87"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="86"/>
       <c r="R14" s="83"/>
       <c r="S14" s="83"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="88"/>
-      <c r="V14" s="88"/>
+      <c r="T14" s="87"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="83"/>
       <c r="W14" s="88"/>
-      <c r="X14" s="84"/>
-      <c r="Y14" s="84"/>
-    </row>
-    <row r="15" spans="2:25">
+      <c r="X14" s="88"/>
+      <c r="Y14" s="88"/>
+      <c r="Z14" s="88"/>
+      <c r="AA14" s="84"/>
+      <c r="AB14" s="84"/>
+    </row>
+    <row r="15" spans="2:28">
       <c r="C15" s="42"/>
       <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="30" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="29" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C18" s="29">
         <v>1368</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="29" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C19" s="97">
-        <f>C18/I58</f>
-        <v>1660.1920877257439</v>
+        <f>C18/G59</f>
+        <v>1812.0956459316621</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="29" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C20" s="29">
         <v>30</v>
@@ -3859,7 +3930,7 @@
         <v>1350</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -3886,143 +3957,143 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:12">
-      <c r="B33" s="30" t="s">
+    <row r="30" spans="2:4">
+      <c r="B30" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
+      <c r="B34" s="29" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="2:12">
-      <c r="B34" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12">
-      <c r="B35" s="29" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12">
+    <row r="35" spans="2:15">
+      <c r="B35" s="89" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15">
       <c r="B36" s="29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
+      <c r="B37" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
       <c r="B39" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="2:12">
+    <row r="40" spans="2:15">
       <c r="B40" s="29" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C40" s="96">
         <v>0.82</v>
       </c>
-      <c r="D40" s="29">
-        <v>1</v>
-      </c>
-      <c r="E40" s="98">
-        <f>D40/SUM($D$40:$D$42)</f>
-        <v>0.82000000000000006</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12">
+      <c r="H40" s="98"/>
+    </row>
+    <row r="41" spans="2:15">
       <c r="B41" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C41" s="96">
         <v>0.15</v>
       </c>
-      <c r="D41" s="90">
-        <f>D$40/$C$40*C41</f>
-        <v>0.18292682926829268</v>
-      </c>
-      <c r="E41" s="98">
-        <f>D41/SUM($D$40:$D$42)</f>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12">
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="90"/>
+      <c r="H41" s="98"/>
+    </row>
+    <row r="42" spans="2:15">
       <c r="B42" s="29" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="96">
         <v>0.03</v>
       </c>
-      <c r="D42" s="90">
-        <f>D$40/$C$40*C42</f>
-        <v>3.6585365853658534E-2</v>
-      </c>
-      <c r="E42" s="98">
-        <f>D42/SUM($D$40:$D$42)</f>
-        <v>0.03</v>
-      </c>
-      <c r="L42" s="29" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12">
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="98"/>
+      <c r="O42" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
       <c r="B45" s="89" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
       <c r="B46" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
       <c r="B47" s="99" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
       <c r="B48" s="99" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20">
       <c r="B49" s="99" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20">
       <c r="B50" s="99" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12">
-      <c r="B52" s="89" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20">
+      <c r="B52" s="149" t="s">
         <v>95</v>
       </c>
-      <c r="C52" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="F52" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="G52" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="H52" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="I52" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12">
+      <c r="C52" s="143" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="143" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="143" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" s="143" t="s">
+        <v>152</v>
+      </c>
+      <c r="G52" s="143" t="s">
+        <v>154</v>
+      </c>
+      <c r="T52" s="128"/>
+    </row>
+    <row r="53" spans="2:20">
       <c r="B53" s="29" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C53" s="29">
         <v>2.3199999999999998</v>
@@ -4031,28 +4102,25 @@
         <f>C53</f>
         <v>2.3199999999999998</v>
       </c>
-      <c r="E53" s="90">
-        <f>D53/$D$58</f>
-        <v>2.2504</v>
+      <c r="E53" s="29">
+        <f>D53*C71</f>
+        <v>46.4</v>
       </c>
       <c r="F53" s="90">
-        <f>E53*C84</f>
-        <v>45.007999999999996</v>
+        <f>E53</f>
+        <v>46.4</v>
       </c>
       <c r="G53" s="90">
-        <f>F53/$C$85</f>
-        <v>1.0430590961761297</v>
-      </c>
-      <c r="H53" s="90">
-        <f>G53/$G$56</f>
-        <v>0.95984365433259322</v>
-      </c>
-      <c r="I53" s="90">
-        <f>H53</f>
-        <v>0.95984365433259322</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12">
+        <f>F53/$F$56</f>
+        <v>0.96028477410542445</v>
+      </c>
+      <c r="H53" s="90"/>
+      <c r="I53" s="90"/>
+      <c r="J53" s="90"/>
+      <c r="K53" s="90"/>
+      <c r="L53" s="90"/>
+    </row>
+    <row r="54" spans="2:20">
       <c r="B54" s="29" t="s">
         <v>83</v>
       </c>
@@ -4063,48 +4131,45 @@
         <f t="shared" ref="D54" si="0">C54</f>
         <v>0.01</v>
       </c>
-      <c r="E54" s="90">
-        <f>D54/$D$58</f>
-        <v>9.700000000000002E-3</v>
+      <c r="E54" s="29">
+        <f>D54*C69</f>
+        <v>1.2010000000000001</v>
       </c>
       <c r="F54" s="90">
-        <f>E54*C82</f>
-        <v>1.1649700000000003</v>
+        <f>E54+E55</f>
+        <v>1.919</v>
       </c>
       <c r="G54" s="90">
-        <f>F54/$C$85</f>
-        <v>2.6998146002317504E-2</v>
-      </c>
-      <c r="H54" s="90">
-        <f>G54/$G$56</f>
-        <v>2.4844229070117348E-2</v>
-      </c>
-      <c r="I54" s="90">
-        <f>H54+H55</f>
-        <v>4.0156345667406765E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12">
-      <c r="B55" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E55" s="90"/>
-      <c r="F55" s="90">
+        <f>F54/$F$56</f>
+        <v>3.9715225894575636E-2</v>
+      </c>
+      <c r="H54" s="90"/>
+      <c r="I54" s="90"/>
+      <c r="J54" s="90"/>
+      <c r="K54" s="90"/>
+      <c r="L54" s="90"/>
+      <c r="T54" s="129"/>
+    </row>
+    <row r="55" spans="2:20">
+      <c r="B55" s="143" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="144"/>
+      <c r="D55" s="144"/>
+      <c r="E55" s="145">
         <v>0.71799999999999997</v>
       </c>
-      <c r="G55" s="90">
-        <f>F55/$C$85</f>
-        <v>1.6639629200463499E-2</v>
-      </c>
-      <c r="H55" s="90">
-        <f>G55/$G$56</f>
-        <v>1.5312116597289415E-2</v>
-      </c>
-      <c r="I55" s="29">
+      <c r="F55" s="146">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:12">
+      <c r="G55" s="147"/>
+      <c r="H55" s="90"/>
+      <c r="I55" s="90"/>
+      <c r="J55" s="90"/>
+      <c r="K55" s="90"/>
+      <c r="T55" s="129"/>
+    </row>
+    <row r="56" spans="2:20">
       <c r="B56" s="29" t="s">
         <v>49</v>
       </c>
@@ -4116,375 +4181,290 @@
         <f>SUM(D53:D54)</f>
         <v>2.3299999999999996</v>
       </c>
-      <c r="E56" s="90">
-        <f>SUM(E53:E54)</f>
-        <v>2.2601</v>
-      </c>
-      <c r="F56" s="90">
+      <c r="E56" s="29">
+        <f>SUM(E53:E55)</f>
+        <v>48.319000000000003</v>
+      </c>
+      <c r="F56" s="29">
         <f>SUM(F53:F55)</f>
-        <v>46.890969999999996</v>
+        <v>48.318999999999996</v>
       </c>
       <c r="G56" s="90">
-        <f>SUM(G53:G55)</f>
-        <v>1.0866968713789107</v>
-      </c>
-      <c r="H56" s="90">
-        <f>SUM(H53:H55)</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="I56" s="90">
-        <f>SUM(I53:I55)</f>
+        <f>F56/F56</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="2:12">
-      <c r="B57" s="89" t="s">
+      <c r="H56" s="90"/>
+      <c r="I56" s="90"/>
+      <c r="J56" s="90"/>
+      <c r="K56" s="90"/>
+      <c r="L56" s="90"/>
+      <c r="T56" s="129"/>
+    </row>
+    <row r="57" spans="2:20">
+      <c r="H57" s="90"/>
+      <c r="I57" s="90"/>
+      <c r="J57" s="90"/>
+      <c r="K57" s="90"/>
+      <c r="T57" s="129"/>
+    </row>
+    <row r="58" spans="2:20">
+      <c r="B58" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="E57" s="90"/>
-      <c r="F57" s="90"/>
-      <c r="G57" s="90"/>
-      <c r="H57" s="90"/>
-    </row>
-    <row r="58" spans="2:12">
-      <c r="B58" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C58" s="29">
-        <f>D40</f>
+      <c r="C58" s="143"/>
+      <c r="D58" s="143"/>
+      <c r="E58" s="143"/>
+      <c r="F58" s="145"/>
+      <c r="G58" s="145"/>
+      <c r="H58" s="90"/>
+      <c r="I58" s="90"/>
+      <c r="J58" s="90"/>
+      <c r="K58" s="90"/>
+      <c r="L58" s="90"/>
+      <c r="O58" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="T58" s="129"/>
+    </row>
+    <row r="59" spans="2:20">
+      <c r="B59" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="130">
+        <f>C40</f>
+        <v>0.82</v>
+      </c>
+      <c r="D59" s="90">
+        <f>C59+$C$61*C59/SUM($C$59:$C$60)</f>
+        <v>0.84536082474226804</v>
+      </c>
+      <c r="E59" s="90">
+        <f>D59*C72</f>
+        <v>36.477319587628863</v>
+      </c>
+      <c r="F59" s="90">
+        <f t="shared" ref="F59:F60" si="1">E59</f>
+        <v>36.477319587628863</v>
+      </c>
+      <c r="G59" s="90">
+        <f>F59/$F$56</f>
+        <v>0.75492703879693013</v>
+      </c>
+      <c r="H59" s="90"/>
+      <c r="I59" s="90"/>
+      <c r="J59" s="90"/>
+      <c r="K59" s="90"/>
+      <c r="L59" s="90"/>
+      <c r="T59" s="129"/>
+    </row>
+    <row r="60" spans="2:20">
+      <c r="B60" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="130">
+        <f>C41</f>
+        <v>0.15</v>
+      </c>
+      <c r="D60" s="90">
+        <f>C60+$C$61*C60/SUM($C$59:$C$60)</f>
+        <v>0.15463917525773196</v>
+      </c>
+      <c r="E60" s="90">
+        <f>D60*C70</f>
+        <v>6.9587628865979383</v>
+      </c>
+      <c r="F60" s="90">
+        <f t="shared" si="1"/>
+        <v>6.9587628865979383</v>
+      </c>
+      <c r="G60" s="90">
+        <f>F60/$F$56</f>
+        <v>0.14401711307348949</v>
+      </c>
+      <c r="H60" s="90"/>
+      <c r="I60" s="90"/>
+      <c r="J60" s="90"/>
+      <c r="K60" s="90"/>
+      <c r="T60" s="129"/>
+    </row>
+    <row r="61" spans="2:20">
+      <c r="B61" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="130">
+        <f>C42</f>
+        <v>0.03</v>
+      </c>
+      <c r="D61" s="29">
+        <v>0</v>
+      </c>
+      <c r="E61" s="140"/>
+      <c r="F61" s="142"/>
+      <c r="G61" s="142"/>
+      <c r="H61" s="90"/>
+      <c r="I61" s="90"/>
+      <c r="J61" s="90"/>
+      <c r="K61" s="90"/>
+      <c r="T61" s="129"/>
+    </row>
+    <row r="62" spans="2:20">
+      <c r="B62" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="140"/>
+      <c r="D62" s="140"/>
+      <c r="E62" s="90">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="F62" s="41">
+        <v>0</v>
+      </c>
+      <c r="G62" s="141"/>
+      <c r="H62" s="90"/>
+      <c r="I62" s="90"/>
+      <c r="J62" s="90"/>
+      <c r="K62" s="90"/>
+      <c r="L62" s="90"/>
+      <c r="T62" s="129"/>
+    </row>
+    <row r="63" spans="2:20">
+      <c r="B63" s="143" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="144"/>
+      <c r="D63" s="144"/>
+      <c r="E63" s="144"/>
+      <c r="F63" s="148"/>
+      <c r="G63" s="145">
+        <f>1-SUM(G59:G62)</f>
+        <v>0.10105584812958035</v>
+      </c>
+      <c r="H63" s="90"/>
+      <c r="I63" s="90"/>
+      <c r="J63" s="90"/>
+      <c r="K63" s="90"/>
+      <c r="L63" s="90"/>
+      <c r="T63" s="129"/>
+    </row>
+    <row r="64" spans="2:20">
+      <c r="B64" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="90">
+        <f>SUM(C59:C61)</f>
         <v>1</v>
       </c>
-      <c r="D58" s="90">
-        <f>C58+$C$60*C58/SUM($C$58:$C$59)</f>
-        <v>1.0309278350515463</v>
-      </c>
-      <c r="E58" s="90">
-        <f>D58/$D$58</f>
+      <c r="D64" s="90">
+        <f>SUM(D59:D61)</f>
         <v>1</v>
       </c>
-      <c r="F58" s="90">
+      <c r="E64" s="90">
+        <f>SUM(E59:E63)</f>
+        <v>44.750082474226801</v>
+      </c>
+      <c r="F64" s="90">
+        <f>SUM(F59:F63)</f>
+        <v>43.436082474226801</v>
+      </c>
+      <c r="G64" s="90">
+        <f>SUM(G59:G63)</f>
         <v>1</v>
       </c>
-      <c r="G58" s="90">
-        <v>1</v>
-      </c>
-      <c r="H58" s="90">
-        <f>G58/$G$63</f>
-        <v>0.82400103585241713</v>
-      </c>
-      <c r="I58" s="90">
-        <f>H58</f>
-        <v>0.82400103585241713</v>
-      </c>
-      <c r="L58" s="29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12">
-      <c r="B59" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="C59" s="90">
-        <f>D41</f>
-        <v>0.18292682926829268</v>
-      </c>
-      <c r="D59" s="90">
-        <f>C59+$C$60*C59/SUM($C$58:$C$59)</f>
-        <v>0.18858436007040483</v>
-      </c>
-      <c r="E59" s="90">
-        <f>D59/$D$58</f>
-        <v>0.18292682926829271</v>
-      </c>
-      <c r="F59" s="90">
-        <f>E59*C83</f>
-        <v>7.9024390243902456</v>
-      </c>
-      <c r="G59" s="90">
-        <f>F59/$C$85</f>
-        <v>0.1831387954667496</v>
-      </c>
-      <c r="H59" s="90">
-        <f>G59/$G$63</f>
-        <v>0.15090655716936563</v>
-      </c>
-      <c r="I59" s="90">
-        <f>H59</f>
-        <v>0.15090655716936563</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12">
-      <c r="B60" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C60" s="90">
-        <f>D42</f>
-        <v>3.6585365853658534E-2</v>
-      </c>
-      <c r="D60" s="29">
-        <v>0</v>
-      </c>
-      <c r="E60" s="90"/>
-      <c r="F60" s="90">
-        <v>0</v>
-      </c>
-      <c r="G60" s="90">
-        <v>0</v>
-      </c>
-      <c r="H60" s="90">
-        <f>G60/$G$63</f>
-        <v>0</v>
-      </c>
-      <c r="I60" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12">
-      <c r="B61" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="E61" s="90"/>
-      <c r="F61" s="90">
-        <v>1.3140000000000001</v>
-      </c>
-      <c r="G61" s="90">
-        <f>F61/$C$85</f>
-        <v>3.0451911935110085E-2</v>
-      </c>
-      <c r="H61" s="90">
-        <f>G61/$G$63</f>
-        <v>2.5092406978217293E-2</v>
-      </c>
-      <c r="I61" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12">
-      <c r="B62" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E62" s="90"/>
-      <c r="F62" s="90"/>
-      <c r="G62" s="90"/>
-      <c r="H62" s="90"/>
-      <c r="I62" s="90">
-        <f>H61</f>
-        <v>2.5092406978217293E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12">
-      <c r="B63" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63" s="90">
-        <f>SUM(C58:C60)</f>
-        <v>1.2195121951219512</v>
-      </c>
-      <c r="D63" s="90">
-        <f>SUM(D58:D60)</f>
-        <v>1.2195121951219512</v>
-      </c>
-      <c r="E63" s="90">
-        <f>SUM(E58:E60)</f>
-        <v>1.1829268292682926</v>
-      </c>
-      <c r="F63" s="90">
-        <f>SUM(F58:F60)</f>
-        <v>8.9024390243902456</v>
-      </c>
-      <c r="G63" s="90">
-        <f>SUM(G58:G61)</f>
-        <v>1.2135907074018597</v>
-      </c>
-      <c r="H63" s="90">
-        <f>SUM(H58:H61)</f>
-        <v>1</v>
-      </c>
-      <c r="I63" s="90">
-        <f>SUM(I58:I62)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5">
-      <c r="B66" s="89" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5">
-      <c r="B67" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5">
-      <c r="C69" s="29" t="s">
-        <v>141</v>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="B66" s="89"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="B69" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="29">
+        <v>120.1</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="E69" s="29" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5">
-      <c r="B70" s="89" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="B70" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" s="29">
+        <v>45</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="B71" s="29" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C71" s="29">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="D71" s="90">
-        <f>C71*C84/$C$85</f>
-        <v>1.0753186558516803</v>
-      </c>
-      <c r="E71" s="37">
-        <f>D71/$D$74</f>
-        <v>0.96028477410542434</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5">
+        <v>20</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E71" s="90"/>
+      <c r="F71" s="90"/>
+      <c r="G71" s="90"/>
+      <c r="H71" s="37"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="B72" s="29" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="C72" s="29">
-        <v>0.01</v>
-      </c>
-      <c r="D72" s="90">
-        <f>C72*C82/$C$85</f>
-        <v>2.783314020857474E-2</v>
-      </c>
-      <c r="E72" s="37">
-        <f>D72/$D$74</f>
-        <v>2.4855646846996003E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5">
-      <c r="B73" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D73" s="90">
-        <f>0.718/$C$85</f>
-        <v>1.6639629200463499E-2</v>
-      </c>
-      <c r="E73" s="37">
-        <f>D73/$D$74</f>
-        <v>1.4859579047579624E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5">
-      <c r="B74" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D74" s="90">
-        <f>SUM(D71:D73)</f>
-        <v>1.1197914252607186</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5">
-      <c r="B75" s="89" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5">
-      <c r="B76" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C76" s="29">
-        <v>1</v>
-      </c>
-      <c r="D76" s="29">
-        <v>1</v>
-      </c>
-      <c r="E76" s="37">
-        <f>D76/$D$78</f>
-        <v>0.97044800287873334</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5">
-      <c r="B77" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="D77" s="90">
-        <f>1.314/$C$85</f>
-        <v>3.0451911935110085E-2</v>
-      </c>
-      <c r="E77" s="37">
-        <f>D77/$D$78</f>
-        <v>2.9551997121266646E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5">
-      <c r="B78" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D78" s="90">
-        <f>SUM(D76:D77)</f>
-        <v>1.0304519119351101</v>
-      </c>
-      <c r="E78" s="29">
-        <f>SUM(E76:E77)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="B82" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C82" s="29">
-        <v>120.1</v>
-      </c>
-      <c r="D82" s="29" t="s">
+        <v>43.15</v>
+      </c>
+      <c r="D72" s="29" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="B83" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="C83" s="29">
-        <v>43.2</v>
-      </c>
-      <c r="D83" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E83" s="29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="B84" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="C84" s="29">
-        <v>20</v>
-      </c>
-      <c r="D84" s="29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="B85" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C85" s="29">
-        <v>43.15</v>
-      </c>
-      <c r="D85" s="29" t="s">
-        <v>84</v>
-      </c>
+      <c r="E72" s="90"/>
+      <c r="F72" s="90"/>
+      <c r="G72" s="90"/>
+      <c r="H72" s="37"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="D73" s="90"/>
+      <c r="E73" s="90"/>
+      <c r="F73" s="90"/>
+      <c r="G73" s="90"/>
+      <c r="H73" s="37"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="D74" s="90"/>
+      <c r="E74" s="90"/>
+      <c r="F74" s="90"/>
+      <c r="G74" s="90"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="B75" s="89"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="H76" s="37"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="D77" s="90"/>
+      <c r="E77" s="90"/>
+      <c r="F77" s="90"/>
+      <c r="G77" s="90"/>
+      <c r="H77" s="37"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="D78" s="90"/>
+      <c r="E78" s="90"/>
+      <c r="F78" s="90"/>
+      <c r="G78" s="90"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>